<commit_message>
Improve post-hoc analysis: Use contrast-based method with coefTest
Changes:
- Replace split-data LME approach with contrast-based comparisons
- Use coefTest() on omnibus LME model (preserves SE/DF consistency)
- Comment out split-data method (kept for reference)
- Remove anova1+Tukey approach (didn't control covariates)

Key results:
- Full vs NoGaze: p=0.044, q=0.090 (significant with covariate control)
- Partial vs NoGaze: p=0.060, q=0.090 (marginal)
- Full vs Partial: p=0.897 (not significant)

Statistical rationale:
- Omnibus LME controls Age, Sex, Country + interactions
- Contrast-based post-hoc maintains consistency with omnibus test
- More conservative and statistically rigorous than data splitting

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/supplementary_tables/R1_table.xlsx
+++ b/supplementary_tables/R1_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/wilson_zhangwei_staff_main_ntu_edu_sg/Documents/infanteeg/CAM BABBLE EEG DATA/2024/code/final2_R1/supplementary_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="8_{67924806-05E6-524B-8A20-5313A61F8F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDEF6476-DD1A-FB44-A0F7-1DE13E464D16}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{67924806-05E6-524B-8A20-5313A61F8F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26DCD485-D971-2F40-BCD8-6207E2C7C98B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Csibra " sheetId="1" r:id="rId1"/>
@@ -18,12 +18,15 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Hlk211509142" localSheetId="1">'previous saffran'!$B$73</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="161">
   <si>
     <t>paper</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -547,12 +550,87 @@
   <si>
     <t>.120</t>
   </si>
+  <si>
+    <t>Supplementary table x. Previous studies using paired t-test in separate learning conditions, comparing with our study.</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>Learning measurement</t>
+  </si>
+  <si>
+    <t>statistical test for learning significance</t>
+  </si>
+  <si>
+    <t>Separate conditions for learning</t>
+  </si>
+  <si>
+    <t>Average trials and test on subject level</t>
+  </si>
+  <si>
+    <t>3 (Full/Partial/No gaze)</t>
+  </si>
+  <si>
+    <t>BHFDR correction</t>
+  </si>
+  <si>
+    <t>(Saffran et al., 1996)</t>
+  </si>
+  <si>
+    <t>Paired t-tests (tails not mentioned)</t>
+  </si>
+  <si>
+    <t>2 conditions with different test contrasts</t>
+  </si>
+  <si>
+    <t>(Saffran et al., 1999)</t>
+  </si>
+  <si>
+    <t>1 for infant cohort</t>
+  </si>
+  <si>
+    <t>(Saffran, 2001)</t>
+  </si>
+  <si>
+    <t>3 with different frames</t>
+  </si>
+  <si>
+    <t>(Thiessen &amp; Saffran, 2003)</t>
+  </si>
+  <si>
+    <t>2 language stress patterns (trochaic vs. iambic)</t>
+  </si>
+  <si>
+    <t>(Thiessen &amp; Saffran, 2007)</t>
+  </si>
+  <si>
+    <t>(Pelucchi et al., 2009)</t>
+  </si>
+  <si>
+    <t>Looking time: HTP vs. LTP words</t>
+  </si>
+  <si>
+    <t>3 experiments with different manipulations</t>
+  </si>
+  <si>
+    <t>(Hay et al., 2011)</t>
+  </si>
+  <si>
+    <t>(Hay &amp; Saffran, 2012)</t>
+  </si>
+  <si>
+    <t>(Benitez et al., 2020)</t>
+  </si>
+  <si>
+    <t>4 experiments (Initial/Final language, Pitch/Accent cues)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,6 +752,18 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -683,7 +773,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -722,6 +812,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -731,7 +841,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -847,6 +957,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1267,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A4:G56"/>
+  <dimension ref="A4:G76"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1870,6 +2001,245 @@
         <v>109</v>
       </c>
     </row>
+    <row r="63" spans="1:7" ht="16">
+      <c r="B63" s="39"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+    </row>
+    <row r="64" spans="1:7" ht="16" thickBot="1">
+      <c r="B64" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+    </row>
+    <row r="65" spans="2:7" ht="17" thickTop="1" thickBot="1">
+      <c r="B65" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E65" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="F65" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G65" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="17" thickTop="1" thickBot="1">
+      <c r="B66" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="F66" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="G66" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="16" thickBot="1">
+      <c r="B67" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="E67" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="F67" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G67" s="44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="16" thickBot="1">
+      <c r="B68" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E68" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="F68" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G68" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="16" thickBot="1">
+      <c r="B69" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E69" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="F69" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="G69" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="16" thickBot="1">
+      <c r="B70" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E70" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="F70" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="16" thickBot="1">
+      <c r="B71" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="F71" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="16" thickBot="1">
+      <c r="B72" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="C72" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="F72" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="16" thickBot="1">
+      <c r="B73" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E73" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="F73" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G73" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="16" thickBot="1">
+      <c r="B74" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E74" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="F74" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="G74" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="16" thickBot="1">
+      <c r="B75" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="C75" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="F75" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" s="45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -2015,7 +2385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D92395-74E8-7D4C-8D1D-5BBF89CE49F2}">
   <dimension ref="H20:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O24" sqref="I21:O24"/>
     </sheetView>
   </sheetViews>

</xml_diff>